<commit_message>
v11.3 Wstęp Teoretyczny, Excel z v i E, brak niepewności  i gęstości
</commit_message>
<xml_diff>
--- a/Lab 5 - Fale podłużne w ciałach stałych/Zeszyt1.xlsx
+++ b/Lab 5 - Fale podłużne w ciałach stałych/Zeszyt1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Nr</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>Nr 4</t>
-  </si>
-  <si>
-    <t>Domnienama prędkość</t>
-  </si>
-  <si>
-    <t>Domniemana częstotliwość</t>
   </si>
   <si>
     <t>Masa pręta [g]</t>
@@ -207,6 +201,42 @@
   <si>
     <t>ALUMINIUM</t>
   </si>
+  <si>
+    <t xml:space="preserve">v średnie = </t>
+  </si>
+  <si>
+    <t>Modół Younga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gęstość = </t>
+  </si>
+  <si>
+    <t>Niepewności</t>
+  </si>
+  <si>
+    <t>u(m) = [g]</t>
+  </si>
+  <si>
+    <t>u(l) = []</t>
+  </si>
+  <si>
+    <t>u(suwmiarka) = []</t>
+  </si>
+  <si>
+    <t>u(objetości) = []</t>
+  </si>
+  <si>
+    <t>u(gęstości) = []</t>
+  </si>
+  <si>
+    <t>u(f) = []</t>
+  </si>
+  <si>
+    <t>u(v) = []</t>
+  </si>
+  <si>
+    <t>u( E ) = []</t>
+  </si>
 </sst>
 </file>
 
@@ -269,7 +299,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -329,11 +359,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,6 +441,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +761,7 @@
     <col min="4" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="12" max="12" width="30.42578125" customWidth="1"/>
@@ -681,22 +793,22 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -728,7 +840,7 @@
     </row>
     <row r="2" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1">
         <v>31</v>
@@ -751,19 +863,19 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K2" s="5">
         <v>66</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -795,7 +907,7 @@
     </row>
     <row r="3" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
         <v>74</v>
@@ -818,19 +930,19 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K3" s="5">
         <v>31</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -862,7 +974,7 @@
     </row>
     <row r="4" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -885,19 +997,19 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="5">
         <v>174</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -929,7 +1041,7 @@
     </row>
     <row r="5" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -952,19 +1064,19 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K5" s="5">
         <v>24</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -996,7 +1108,7 @@
     </row>
     <row r="6" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -1086,7 +1198,7 @@
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1129,7 +1241,7 @@
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1140,12 +1252,18 @@
         <v>1.8</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8730.7900000000009</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1180,7 +1298,7 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
     </row>
-    <row r="10" spans="1:41" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1193,12 +1311,10 @@
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1250,11 +1366,13 @@
         <f>C11*B11</f>
         <v>3712.5</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="10"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1303,11 +1421,13 @@
         <f t="shared" ref="D12:D16" si="2">C12*B12</f>
         <v>3712.5</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1356,11 +1476,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="11"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1409,11 +1531,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="11"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1462,11 +1586,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="11"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1515,11 +1641,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="11"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1556,13 +1684,23 @@
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1">
+        <f>AVERAGE(D11:D16)</f>
+        <v>3712.5</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" ref="E12:E17" si="3">$F$9*D17*D17</f>
+        <v>120333477360.93752</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="11"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1596,7 +1734,7 @@
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1604,8 +1742,10 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="12"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1650,10 +1790,14 @@
         <v>1.8</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8037.33</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1703,12 +1847,10 @@
       <c r="D20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1750,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>1429.6880000000001</v>
+        <v>1429.69</v>
       </c>
       <c r="C21" s="1">
         <f>2*C19</f>
@@ -1758,9 +1900,9 @@
       </c>
       <c r="D21" s="1">
         <f>C21*B21</f>
-        <v>5146.8768000000009</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>5146.884</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1802,16 +1944,18 @@
       <c r="A22" s="1">
         <v>2</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>2859.38</v>
+      </c>
       <c r="C22" s="1">
         <f>C19</f>
         <v>1.8</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:D26" si="3">C22*B22</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="1"/>
+        <f t="shared" ref="D22:D26" si="4">C22*B22</f>
+        <v>5146.884</v>
+      </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1853,16 +1997,18 @@
       <c r="A23" s="1">
         <v>3</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>4289.0600000000004</v>
+      </c>
       <c r="C23" s="1">
         <f>C19*2/3</f>
         <v>1.2</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
+        <f t="shared" si="4"/>
+        <v>5146.8720000000003</v>
+      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1904,16 +2050,18 @@
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>5742.19</v>
+      </c>
       <c r="C24" s="1">
         <f>C19*2/4</f>
         <v>0.9</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="1"/>
+        <f t="shared" si="4"/>
+        <v>5167.9709999999995</v>
+      </c>
+      <c r="E24" s="8"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1955,16 +2103,18 @@
       <c r="A25" s="1">
         <v>5</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>7171.88</v>
+      </c>
       <c r="C25" s="1">
         <f>C19*2/5</f>
         <v>0.72</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
+        <f t="shared" si="4"/>
+        <v>5163.7536</v>
+      </c>
+      <c r="E25" s="8"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2006,16 +2156,18 @@
       <c r="A26" s="1">
         <v>6</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>8601.56</v>
+      </c>
       <c r="C26" s="1">
         <f>C19*2/6</f>
         <v>0.6</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="1"/>
+        <f t="shared" si="4"/>
+        <v>5160.9359999999997</v>
+      </c>
+      <c r="E26" s="8"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2056,9 +2208,17 @@
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1">
+        <f>AVERAGE(D21:D26)</f>
+        <v>5155.5500999999995</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" ref="E22:E27" si="5">$F$19*D27*D27</f>
+        <v>213629794751.67868</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2150,10 +2310,14 @@
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="1">
+        <v>8708.7099999999991</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2203,12 +2367,10 @@
       <c r="D30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2249,16 +2411,18 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1">
+        <v>1710.94</v>
+      </c>
       <c r="C31" s="1">
         <f>2*C29</f>
         <v>2</v>
       </c>
       <c r="D31" s="1">
         <f>C31*B31</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>3421.88</v>
+      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2300,16 +2464,18 @@
       <c r="A32" s="1">
         <v>2</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>3445.31</v>
+      </c>
       <c r="C32" s="1">
         <f>C29</f>
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" ref="D32:D36" si="4">C32*B32</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="1"/>
+        <f t="shared" ref="D32:D36" si="6">C32*B32</f>
+        <v>3445.31</v>
+      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2351,16 +2517,18 @@
       <c r="A33" s="1">
         <v>3</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1">
+        <v>5156.25</v>
+      </c>
       <c r="C33" s="1">
         <f>C29*2/3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="1"/>
+        <f t="shared" si="6"/>
+        <v>3437.5</v>
+      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2402,16 +2570,18 @@
       <c r="A34" s="1">
         <v>4</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1">
+        <v>6890.63</v>
+      </c>
       <c r="C34" s="1">
         <f>C29*2/4</f>
         <v>0.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="1"/>
+        <f t="shared" si="6"/>
+        <v>3445.3150000000001</v>
+      </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2453,16 +2623,18 @@
       <c r="A35" s="1">
         <v>5</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1">
+        <v>8601.56</v>
+      </c>
       <c r="C35" s="1">
         <f>C29*2/5</f>
         <v>0.4</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="1"/>
+        <f t="shared" si="6"/>
+        <v>3440.6239999999998</v>
+      </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2501,19 +2673,19 @@
       <c r="AO35" s="1"/>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>6</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1">
-        <f>C29*2/6</f>
-        <v>0.33333333333333331</v>
+      <c r="C36" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="1"/>
+        <f>AVERAGE(D31:D35)</f>
+        <v>3438.1258000000003</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" ref="E32:E36" si="7">$F$29*D36*D36</f>
+        <v>102943126820.17787</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2648,10 +2820,14 @@
         <v>1</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2777.98</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2701,12 +2877,10 @@
       <c r="D40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E40" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2747,16 +2921,18 @@
       <c r="A41" s="1">
         <v>1</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1">
+        <v>2460.94</v>
+      </c>
       <c r="C41" s="1">
         <f>2*C39</f>
         <v>2</v>
       </c>
       <c r="D41" s="1">
         <f>C41*B41</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>4921.88</v>
+      </c>
+      <c r="E41" s="8"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2798,16 +2974,18 @@
       <c r="A42" s="1">
         <v>2</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1">
+        <v>4945.3100000000004</v>
+      </c>
       <c r="C42" s="1">
         <f>C39</f>
         <v>1</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" ref="D42:D46" si="5">C42*B42</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="1"/>
+        <f t="shared" ref="D42:D46" si="8">C42*B42</f>
+        <v>4945.3100000000004</v>
+      </c>
+      <c r="E42" s="8"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -2849,16 +3027,18 @@
       <c r="A43" s="1">
         <v>3</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1">
+        <v>7406.25</v>
+      </c>
       <c r="C43" s="1">
         <f>C39*2/3</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="1"/>
+        <f t="shared" si="8"/>
+        <v>4937.5</v>
+      </c>
+      <c r="E43" s="8"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -2900,16 +3080,18 @@
       <c r="A44" s="1">
         <v>4</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1">
+        <v>9867.19</v>
+      </c>
       <c r="C44" s="1">
         <f>C39*2/4</f>
         <v>0.5</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="1"/>
+        <f t="shared" si="8"/>
+        <v>4933.5950000000003</v>
+      </c>
+      <c r="E44" s="8"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2948,19 +3130,19 @@
       <c r="AO44" s="1"/>
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>5</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="1">
-        <f>C39*2/5</f>
-        <v>0.4</v>
+      <c r="C45" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="1"/>
+        <f>AVERAGE(D41:D44)</f>
+        <v>4934.57125</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" ref="E42:E45" si="9">$F$39*D45*D45</f>
+        <v>67643794724.576759</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2999,18 +3181,10 @@
       <c r="AO45" s="1"/>
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>6</v>
-      </c>
+      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="1">
-        <f>C39*2/6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -5200,6 +5374,12 @@
       <c r="AO96" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E40:E44"/>
+    <mergeCell ref="E30:E35"/>
+    <mergeCell ref="E20:E26"/>
+    <mergeCell ref="E10:E16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
v11.4 Dodane "poprawne" gęstości
</commit_message>
<xml_diff>
--- a/Lab 5 - Fale podłużne w ciałach stałych/Zeszyt1.xlsx
+++ b/Lab 5 - Fale podłużne w ciałach stałych/Zeszyt1.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
-  <si>
-    <t>Nr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Materiał</t>
   </si>
@@ -217,12 +214,6 @@
     <t>u(m) = [g]</t>
   </si>
   <si>
-    <t>u(l) = []</t>
-  </si>
-  <si>
-    <t>u(suwmiarka) = []</t>
-  </si>
-  <si>
     <t>u(objetości) = []</t>
   </si>
   <si>
@@ -236,13 +227,55 @@
   </si>
   <si>
     <t>u( E ) = []</t>
+  </si>
+  <si>
+    <t>u(suwmiarka) = [mm]</t>
+  </si>
+  <si>
+    <t>Wymiary</t>
+  </si>
+  <si>
+    <t>mosiadz</t>
+  </si>
+  <si>
+    <t>a[mm]</t>
+  </si>
+  <si>
+    <t>b[mm]</t>
+  </si>
+  <si>
+    <t>h[mm]</t>
+  </si>
+  <si>
+    <t>Masa[g]</t>
+  </si>
+  <si>
+    <t>Objętość[cm^3</t>
+  </si>
+  <si>
+    <t>Gęstość[kg/m^3]</t>
+  </si>
+  <si>
+    <t>Pole przekroju [mm^2]</t>
+  </si>
+  <si>
+    <t>u(linijka) = [mm]</t>
+  </si>
+  <si>
+    <t>NIE!!!!!!</t>
+  </si>
+  <si>
+    <t>O ta tabelka gęstości</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,16 +323,31 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -360,6 +408,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -371,12 +430,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -416,26 +495,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -449,24 +558,94 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -747,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO96"/>
+  <dimension ref="A1:AP96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,51 +946,54 @@
     <col min="12" max="12" width="30.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:42" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -837,48 +1019,49 @@
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
-    </row>
-    <row r="2" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="AP1" s="1"/>
+    </row>
+    <row r="2" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="29">
         <v>31</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="29">
         <v>4.0124370000000003</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="29">
         <f>B2/C2</f>
         <v>7.7259780028945002</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="29">
         <f>D2*1000</f>
         <v>7725.9780028945006</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29">
         <v>180</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="33">
+        <v>66</v>
+      </c>
+      <c r="L2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="5">
-        <v>66</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -904,48 +1087,49 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
-    </row>
-    <row r="3" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="AP2" s="1"/>
+    </row>
+    <row r="3" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="29">
         <v>74</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="29">
         <v>10.037012000000001</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="29">
         <f t="shared" ref="D3:D6" si="0">B3/C3</f>
         <v>7.3727121179091943</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="29">
         <f t="shared" ref="E3:E6" si="1">D3*1000</f>
         <v>7372.7121179091946</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29">
         <v>99.8</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="33">
+        <v>31</v>
+      </c>
+      <c r="L3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="5">
-        <v>31</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -971,48 +1155,49 @@
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
-    </row>
-    <row r="4" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="AP3" s="1"/>
+    </row>
+    <row r="4" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="29">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="29">
         <v>1.59436</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="29">
         <f t="shared" si="0"/>
         <v>7.526531021852028</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="29">
         <f t="shared" si="1"/>
         <v>7526.5310218520281</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29">
         <v>180</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="33">
+        <v>174</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="5">
-        <v>174</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1038,48 +1223,49 @@
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
-    </row>
-    <row r="5" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="AP4" s="1"/>
+    </row>
+    <row r="5" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="29">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="29">
         <v>0.70799999999999996</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="29">
         <f t="shared" si="0"/>
         <v>7.0621468926553677</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="29">
         <f t="shared" si="1"/>
         <v>7062.146892655368</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1">
+      <c r="F5" s="29"/>
+      <c r="G5" s="29">
         <v>180.1</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="33">
+        <v>24</v>
+      </c>
+      <c r="L5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="5">
-        <v>24</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1105,34 +1291,39 @@
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
-    </row>
-    <row r="6" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="AP5" s="1"/>
+    </row>
+    <row r="6" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="29">
         <v>30</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="29">
         <v>15.748799999999999</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="29">
         <f t="shared" si="0"/>
         <v>1.9049070405364219</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="29">
         <f t="shared" si="1"/>
         <v>1904.9070405364218</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
+      <c r="F6" s="29"/>
+      <c r="G6" s="29">
         <v>99.9</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="6"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -1158,8 +1349,9 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
-    </row>
-    <row r="7" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AP6" s="1"/>
+    </row>
+    <row r="7" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1169,7 +1361,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="6"/>
+      <c r="J7" s="2"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1197,8 +1389,9 @@
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
-    </row>
-    <row r="8" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP7" s="1"/>
+    </row>
+    <row r="8" spans="1:42" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1208,15 +1401,17 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="J8" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -1240,40 +1435,54 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
-    </row>
-    <row r="9" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP8" s="1"/>
+    </row>
+    <row r="9" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>1.8</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>37</v>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="27">
+        <f>$R$11</f>
+        <v>8886.15098929749</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" s="1">
-        <v>8730.7900000000009</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="K9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1297,36 +1506,43 @@
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
-    </row>
-    <row r="10" spans="1:41" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP9" s="1"/>
+    </row>
+    <row r="10" spans="1:42" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>43</v>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="18"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1350,8 +1566,9 @@
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP10" s="1"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1366,22 +1583,41 @@
         <f>C11*B11</f>
         <v>3712.5</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="10"/>
+      <c r="H11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="K11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="20">
+        <v>67</v>
+      </c>
+      <c r="M11" s="13">
+        <v>5</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="20">
+        <v>384</v>
+      </c>
+      <c r="P11" s="20">
+        <f>(M11/2)^2*PI()</f>
+        <v>19.634954084936208</v>
+      </c>
+      <c r="Q11" s="20">
+        <f>O11*P11*10^(-3)</f>
+        <v>7.5398223686155035</v>
+      </c>
+      <c r="R11" s="25">
+        <f>(L11*10^(-3))/(Q11*10^(-6))</f>
+        <v>8886.15098929749</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1405,8 +1641,9 @@
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP11" s="1"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1421,22 +1658,43 @@
         <f t="shared" ref="D12:D16" si="2">C12*B12</f>
         <v>3712.5</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="11"/>
+      <c r="H12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="K12" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="20">
+        <v>33</v>
+      </c>
+      <c r="M12" s="20">
+        <v>14.4</v>
+      </c>
+      <c r="N12" s="20">
+        <v>13.9</v>
+      </c>
+      <c r="O12" s="20">
+        <v>20</v>
+      </c>
+      <c r="P12" s="20">
+        <f>M12*N12</f>
+        <v>200.16</v>
+      </c>
+      <c r="Q12" s="20">
+        <f>O12*P12*10^(-3)</f>
+        <v>4.0031999999999996</v>
+      </c>
+      <c r="R12" s="25">
+        <f t="shared" ref="R12:R13" si="3">(L12*10^(-3))/(Q12*10^(-6))</f>
+        <v>8243.4052757793779</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1460,8 +1718,9 @@
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP12" s="1"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1476,22 +1735,43 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="11"/>
+      <c r="H13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.1</v>
+      </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="K13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="20">
+        <v>175</v>
+      </c>
+      <c r="M13" s="20">
+        <v>10</v>
+      </c>
+      <c r="N13" s="20">
+        <v>9.1</v>
+      </c>
+      <c r="O13" s="20">
+        <v>220</v>
+      </c>
+      <c r="P13" s="20">
+        <f>M13*N13</f>
+        <v>91</v>
+      </c>
+      <c r="Q13" s="20">
+        <f>O13*P13*10^(-3)</f>
+        <v>20.02</v>
+      </c>
+      <c r="R13" s="25">
+        <f t="shared" si="3"/>
+        <v>8741.2587412587436</v>
+      </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
@@ -1515,8 +1795,9 @@
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP13" s="1"/>
+    </row>
+    <row r="14" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1531,22 +1812,39 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="11"/>
+      <c r="H14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="7"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="K14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="17">
+        <v>24</v>
+      </c>
+      <c r="M14" s="16">
+        <v>5</v>
+      </c>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17">
+        <v>438</v>
+      </c>
+      <c r="P14" s="17">
+        <f>(M14/2)^2*PI()</f>
+        <v>19.634954084936208</v>
+      </c>
+      <c r="Q14" s="17">
+        <f>O14*P14*10^(-3)</f>
+        <v>8.6001098892020575</v>
+      </c>
+      <c r="R14" s="26">
+        <f>(L14*10^(-3))/(Q14*10^(-6))</f>
+        <v>2790.6620158578912</v>
+      </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -1570,8 +1868,9 @@
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP14" s="1"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1586,13 +1885,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="11"/>
+      <c r="H15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="7"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1625,8 +1924,9 @@
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP15" s="1"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -1641,13 +1941,13 @@
         <f t="shared" si="2"/>
         <v>3712.5</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="11"/>
+      <c r="H16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="7"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1680,27 +1980,28 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP16" s="1"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1">
         <f>AVERAGE(D11:D16)</f>
         <v>3712.5</v>
       </c>
-      <c r="E17" s="7">
-        <f t="shared" ref="E12:E17" si="3">$F$9*D17*D17</f>
-        <v>120333477360.93752</v>
+      <c r="E17" s="3">
+        <f t="shared" ref="E17" si="4">$F$9*D17*D17</f>
+        <v>122474764471.08473</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="11"/>
+      <c r="H17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="7"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1709,7 +2010,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1733,8 +2034,9 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
-    </row>
-    <row r="18" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP17" s="1"/>
+    </row>
+    <row r="18" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1742,10 +2044,10 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="12"/>
+      <c r="H18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="8"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1778,25 +2080,27 @@
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP18" s="1"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1">
         <v>1.8</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>39</v>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="1">
-        <v>8037.33</v>
+        <v>43</v>
+      </c>
+      <c r="F19" s="27">
+        <f>$R$12</f>
+        <v>8243.4052757793779</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1833,22 +2137,23 @@
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
-    </row>
-    <row r="20" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+      <c r="AP19" s="1"/>
+    </row>
+    <row r="20" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>43</v>
+      <c r="E20" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1886,8 +2191,9 @@
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP20" s="1"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1902,7 +2208,7 @@
         <f>C21*B21</f>
         <v>5146.884</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1939,8 +2245,9 @@
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP21" s="1"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1952,10 +2259,10 @@
         <v>1.8</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" ref="D22:D26" si="4">C22*B22</f>
+        <f t="shared" ref="D22:D26" si="5">C22*B22</f>
         <v>5146.884</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1992,8 +2299,9 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
-    </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP22" s="1"/>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -2005,10 +2313,10 @@
         <v>1.2</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5146.8720000000003</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2045,8 +2353,9 @@
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
-    </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP23" s="1"/>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -2058,10 +2367,10 @@
         <v>0.9</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5167.9709999999995</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2098,8 +2407,9 @@
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
-    </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP24" s="1"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -2111,10 +2421,10 @@
         <v>0.72</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5163.7536</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="4"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2151,8 +2461,9 @@
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
-    </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP25" s="1"/>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -2164,10 +2475,10 @@
         <v>0.6</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5160.9359999999997</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2204,20 +2515,21 @@
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP26" s="1"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1">
         <f>AVERAGE(D21:D26)</f>
         <v>5155.5500999999995</v>
       </c>
-      <c r="E27" s="7">
-        <f t="shared" ref="E22:E27" si="5">$F$19*D27*D27</f>
-        <v>213629794751.67868</v>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27" si="6">$F$19*D27*D27</f>
+        <v>219107213106.79715</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2255,8 +2567,9 @@
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP27" s="1"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2298,25 +2611,27 @@
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
-    </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP28" s="1"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>40</v>
+      <c r="D29" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="1">
-        <v>8708.7099999999991</v>
+        <v>43</v>
+      </c>
+      <c r="F29" s="27">
+        <f>$R$13</f>
+        <v>8741.2587412587436</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2353,22 +2668,23 @@
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
-    </row>
-    <row r="30" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+      <c r="AP29" s="1"/>
+    </row>
+    <row r="30" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>43</v>
+      <c r="E30" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2406,8 +2722,9 @@
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
-    </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP30" s="1"/>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -2422,7 +2739,7 @@
         <f>C31*B31</f>
         <v>3421.88</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2459,8 +2776,9 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
-    </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP31" s="1"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -2472,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" ref="D32:D36" si="6">C32*B32</f>
+        <f t="shared" ref="D32:D36" si="7">C32*B32</f>
         <v>3445.31</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="4"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2512,8 +2830,9 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
       <c r="AO32" s="1"/>
-    </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP32" s="1"/>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -2525,10 +2844,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3437.5</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2565,8 +2884,9 @@
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
-    </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP33" s="1"/>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -2578,10 +2898,10 @@
         <v>0.5</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3445.3150000000001</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2618,8 +2938,9 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
-    </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP34" s="1"/>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>5</v>
       </c>
@@ -2631,10 +2952,10 @@
         <v>0.4</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3440.6239999999998</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2671,20 +2992,21 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
-    </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP35" s="1"/>
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="1">
         <f>AVERAGE(D31:D35)</f>
         <v>3438.1258000000003</v>
       </c>
-      <c r="E36" s="7">
-        <f t="shared" ref="E32:E36" si="7">$F$29*D36*D36</f>
-        <v>102943126820.17787</v>
+      <c r="E36" s="3">
+        <f t="shared" ref="E36" si="8">$F$29*D36*D36</f>
+        <v>103327876019.45494</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2722,8 +3044,9 @@
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
-    </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP36" s="1"/>
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2765,8 +3088,9 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
-    </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP37" s="1"/>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2808,25 +3132,27 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
-    </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP38" s="1"/>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>41</v>
+      <c r="D39" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2777.98</v>
+        <v>43</v>
+      </c>
+      <c r="F39" s="27">
+        <f>$R$14</f>
+        <v>2790.6620158578912</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2863,22 +3189,23 @@
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
-    </row>
-    <row r="40" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+      <c r="AP39" s="1"/>
+    </row>
+    <row r="40" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>43</v>
+      <c r="E40" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2916,8 +3243,9 @@
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
       <c r="AO40" s="1"/>
-    </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP40" s="1"/>
+    </row>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2932,7 +3260,7 @@
         <f>C41*B41</f>
         <v>4921.88</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2969,8 +3297,9 @@
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
       <c r="AO41" s="1"/>
-    </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP41" s="1"/>
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -2982,10 +3311,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" ref="D42:D46" si="8">C42*B42</f>
+        <f t="shared" ref="D42:D46" si="9">C42*B42</f>
         <v>4945.3100000000004</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="4"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -3022,8 +3351,9 @@
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
       <c r="AO42" s="1"/>
-    </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP42" s="1"/>
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -3035,10 +3365,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4937.5</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3075,8 +3405,9 @@
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
       <c r="AO43" s="1"/>
-    </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP43" s="1"/>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4</v>
       </c>
@@ -3088,10 +3419,10 @@
         <v>0.5</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4933.5950000000003</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3128,20 +3459,21 @@
       <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
       <c r="AO44" s="1"/>
-    </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP44" s="1"/>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" s="1">
         <f>AVERAGE(D41:D44)</f>
         <v>4934.57125</v>
       </c>
-      <c r="E45" s="7">
-        <f t="shared" ref="E42:E45" si="9">$F$39*D45*D45</f>
-        <v>67643794724.576759</v>
+      <c r="E45" s="3">
+        <f t="shared" ref="E45" si="10">$F$39*D45*D45</f>
+        <v>67952601727.285568</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -3179,8 +3511,9 @@
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
       <c r="AO45" s="1"/>
-    </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP45" s="1"/>
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3222,8 +3555,9 @@
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
-    </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP46" s="1"/>
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3265,8 +3599,9 @@
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
-    </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP47" s="1"/>
+    </row>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3308,8 +3643,9 @@
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
-    </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP48" s="1"/>
+    </row>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3351,8 +3687,9 @@
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
-    </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP49" s="1"/>
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3394,8 +3731,9 @@
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
-    </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP50" s="1"/>
+    </row>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3437,8 +3775,9 @@
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
-    </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP51" s="1"/>
+    </row>
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3480,8 +3819,9 @@
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
-    </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP52" s="1"/>
+    </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3523,8 +3863,9 @@
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
-    </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP53" s="1"/>
+    </row>
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3566,8 +3907,9 @@
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
-    </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP54" s="1"/>
+    </row>
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3609,8 +3951,9 @@
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
       <c r="AO55" s="1"/>
-    </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP55" s="1"/>
+    </row>
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3652,8 +3995,9 @@
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
-    </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP56" s="1"/>
+    </row>
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3695,8 +4039,9 @@
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
       <c r="AO57" s="1"/>
-    </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP57" s="1"/>
+    </row>
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3738,8 +4083,9 @@
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
       <c r="AO58" s="1"/>
-    </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP58" s="1"/>
+    </row>
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3781,8 +4127,9 @@
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
       <c r="AO59" s="1"/>
-    </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP59" s="1"/>
+    </row>
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3824,8 +4171,9 @@
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
       <c r="AO60" s="1"/>
-    </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP60" s="1"/>
+    </row>
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3867,8 +4215,9 @@
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
-    </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP61" s="1"/>
+    </row>
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3910,8 +4259,9 @@
       <c r="AM62" s="1"/>
       <c r="AN62" s="1"/>
       <c r="AO62" s="1"/>
-    </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP62" s="1"/>
+    </row>
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3953,8 +4303,9 @@
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
       <c r="AO63" s="1"/>
-    </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP63" s="1"/>
+    </row>
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3996,8 +4347,9 @@
       <c r="AM64" s="1"/>
       <c r="AN64" s="1"/>
       <c r="AO64" s="1"/>
-    </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP64" s="1"/>
+    </row>
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4039,8 +4391,9 @@
       <c r="AM65" s="1"/>
       <c r="AN65" s="1"/>
       <c r="AO65" s="1"/>
-    </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP65" s="1"/>
+    </row>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4082,8 +4435,9 @@
       <c r="AM66" s="1"/>
       <c r="AN66" s="1"/>
       <c r="AO66" s="1"/>
-    </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP66" s="1"/>
+    </row>
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4125,8 +4479,9 @@
       <c r="AM67" s="1"/>
       <c r="AN67" s="1"/>
       <c r="AO67" s="1"/>
-    </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP67" s="1"/>
+    </row>
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4168,8 +4523,9 @@
       <c r="AM68" s="1"/>
       <c r="AN68" s="1"/>
       <c r="AO68" s="1"/>
-    </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP68" s="1"/>
+    </row>
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4211,8 +4567,9 @@
       <c r="AM69" s="1"/>
       <c r="AN69" s="1"/>
       <c r="AO69" s="1"/>
-    </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP69" s="1"/>
+    </row>
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4254,8 +4611,9 @@
       <c r="AM70" s="1"/>
       <c r="AN70" s="1"/>
       <c r="AO70" s="1"/>
-    </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP70" s="1"/>
+    </row>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4297,8 +4655,9 @@
       <c r="AM71" s="1"/>
       <c r="AN71" s="1"/>
       <c r="AO71" s="1"/>
-    </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP71" s="1"/>
+    </row>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4340,8 +4699,9 @@
       <c r="AM72" s="1"/>
       <c r="AN72" s="1"/>
       <c r="AO72" s="1"/>
-    </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP72" s="1"/>
+    </row>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4383,8 +4743,9 @@
       <c r="AM73" s="1"/>
       <c r="AN73" s="1"/>
       <c r="AO73" s="1"/>
-    </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP73" s="1"/>
+    </row>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4426,8 +4787,9 @@
       <c r="AM74" s="1"/>
       <c r="AN74" s="1"/>
       <c r="AO74" s="1"/>
-    </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP74" s="1"/>
+    </row>
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4469,8 +4831,9 @@
       <c r="AM75" s="1"/>
       <c r="AN75" s="1"/>
       <c r="AO75" s="1"/>
-    </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP75" s="1"/>
+    </row>
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4512,8 +4875,9 @@
       <c r="AM76" s="1"/>
       <c r="AN76" s="1"/>
       <c r="AO76" s="1"/>
-    </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP76" s="1"/>
+    </row>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4555,8 +4919,9 @@
       <c r="AM77" s="1"/>
       <c r="AN77" s="1"/>
       <c r="AO77" s="1"/>
-    </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP77" s="1"/>
+    </row>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4598,8 +4963,9 @@
       <c r="AM78" s="1"/>
       <c r="AN78" s="1"/>
       <c r="AO78" s="1"/>
-    </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP78" s="1"/>
+    </row>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4641,8 +5007,9 @@
       <c r="AM79" s="1"/>
       <c r="AN79" s="1"/>
       <c r="AO79" s="1"/>
-    </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP79" s="1"/>
+    </row>
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4684,8 +5051,9 @@
       <c r="AM80" s="1"/>
       <c r="AN80" s="1"/>
       <c r="AO80" s="1"/>
-    </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP80" s="1"/>
+    </row>
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4727,8 +5095,9 @@
       <c r="AM81" s="1"/>
       <c r="AN81" s="1"/>
       <c r="AO81" s="1"/>
-    </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP81" s="1"/>
+    </row>
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4770,8 +5139,9 @@
       <c r="AM82" s="1"/>
       <c r="AN82" s="1"/>
       <c r="AO82" s="1"/>
-    </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP82" s="1"/>
+    </row>
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4813,8 +5183,9 @@
       <c r="AM83" s="1"/>
       <c r="AN83" s="1"/>
       <c r="AO83" s="1"/>
-    </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP83" s="1"/>
+    </row>
+    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4856,8 +5227,9 @@
       <c r="AM84" s="1"/>
       <c r="AN84" s="1"/>
       <c r="AO84" s="1"/>
-    </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP84" s="1"/>
+    </row>
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4899,8 +5271,9 @@
       <c r="AM85" s="1"/>
       <c r="AN85" s="1"/>
       <c r="AO85" s="1"/>
-    </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP85" s="1"/>
+    </row>
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4942,8 +5315,9 @@
       <c r="AM86" s="1"/>
       <c r="AN86" s="1"/>
       <c r="AO86" s="1"/>
-    </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP86" s="1"/>
+    </row>
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4985,8 +5359,9 @@
       <c r="AM87" s="1"/>
       <c r="AN87" s="1"/>
       <c r="AO87" s="1"/>
-    </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP87" s="1"/>
+    </row>
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5028,8 +5403,9 @@
       <c r="AM88" s="1"/>
       <c r="AN88" s="1"/>
       <c r="AO88" s="1"/>
-    </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP88" s="1"/>
+    </row>
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5071,8 +5447,9 @@
       <c r="AM89" s="1"/>
       <c r="AN89" s="1"/>
       <c r="AO89" s="1"/>
-    </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP89" s="1"/>
+    </row>
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5114,8 +5491,9 @@
       <c r="AM90" s="1"/>
       <c r="AN90" s="1"/>
       <c r="AO90" s="1"/>
-    </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP90" s="1"/>
+    </row>
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5157,8 +5535,9 @@
       <c r="AM91" s="1"/>
       <c r="AN91" s="1"/>
       <c r="AO91" s="1"/>
-    </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP91" s="1"/>
+    </row>
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5200,8 +5579,9 @@
       <c r="AM92" s="1"/>
       <c r="AN92" s="1"/>
       <c r="AO92" s="1"/>
-    </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP92" s="1"/>
+    </row>
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5243,8 +5623,9 @@
       <c r="AM93" s="1"/>
       <c r="AN93" s="1"/>
       <c r="AO93" s="1"/>
-    </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP93" s="1"/>
+    </row>
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5286,8 +5667,9 @@
       <c r="AM94" s="1"/>
       <c r="AN94" s="1"/>
       <c r="AO94" s="1"/>
-    </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP94" s="1"/>
+    </row>
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5329,8 +5711,9 @@
       <c r="AM95" s="1"/>
       <c r="AN95" s="1"/>
       <c r="AO95" s="1"/>
-    </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP95" s="1"/>
+    </row>
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5372,13 +5755,23 @@
       <c r="AM96" s="1"/>
       <c r="AN96" s="1"/>
       <c r="AO96" s="1"/>
+      <c r="AP96" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="13">
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="J8:R8"/>
     <mergeCell ref="E40:E44"/>
     <mergeCell ref="E30:E35"/>
     <mergeCell ref="E20:E26"/>
     <mergeCell ref="E10:E16"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>